<commit_message>
in views daily weekly monthly message have been corrected
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -451,7 +451,7 @@
     </row>
     <row r="2">
       <c r="A2" s="2" t="n">
-        <v>44746</v>
+        <v>44755</v>
       </c>
       <c r="B2" t="n">
         <v>0</v>
@@ -459,7 +459,7 @@
     </row>
     <row r="3">
       <c r="A3" s="2" t="n">
-        <v>44746.04166666666</v>
+        <v>44755.04166666666</v>
       </c>
       <c r="B3" t="n">
         <v>0</v>
@@ -467,7 +467,7 @@
     </row>
     <row r="4">
       <c r="A4" s="2" t="n">
-        <v>44746.08333333334</v>
+        <v>44755.08333333334</v>
       </c>
       <c r="B4" t="n">
         <v>0</v>
@@ -475,7 +475,7 @@
     </row>
     <row r="5">
       <c r="A5" s="2" t="n">
-        <v>44746.125</v>
+        <v>44755.125</v>
       </c>
       <c r="B5" t="n">
         <v>0</v>
@@ -483,7 +483,7 @@
     </row>
     <row r="6">
       <c r="A6" s="2" t="n">
-        <v>44746.16666666666</v>
+        <v>44755.16666666666</v>
       </c>
       <c r="B6" t="n">
         <v>0</v>
@@ -491,7 +491,7 @@
     </row>
     <row r="7">
       <c r="A7" s="2" t="n">
-        <v>44746.20833333334</v>
+        <v>44755.20833333334</v>
       </c>
       <c r="B7" t="n">
         <v>0</v>
@@ -499,7 +499,7 @@
     </row>
     <row r="8">
       <c r="A8" s="2" t="n">
-        <v>44746.25</v>
+        <v>44755.25</v>
       </c>
       <c r="B8" t="n">
         <v>0</v>
@@ -507,7 +507,7 @@
     </row>
     <row r="9">
       <c r="A9" s="2" t="n">
-        <v>44746.29166666666</v>
+        <v>44755.29166666666</v>
       </c>
       <c r="B9" t="n">
         <v>0</v>
@@ -515,7 +515,7 @@
     </row>
     <row r="10">
       <c r="A10" s="2" t="n">
-        <v>44746.33333333334</v>
+        <v>44755.33333333334</v>
       </c>
       <c r="B10" t="n">
         <v>0</v>
@@ -523,7 +523,7 @@
     </row>
     <row r="11">
       <c r="A11" s="2" t="n">
-        <v>44746.375</v>
+        <v>44755.375</v>
       </c>
       <c r="B11" t="n">
         <v>0</v>
@@ -531,23 +531,23 @@
     </row>
     <row r="12">
       <c r="A12" s="2" t="n">
-        <v>44746.41666666666</v>
+        <v>44755.41666666666</v>
       </c>
       <c r="B12" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="2" t="n">
-        <v>44746.45833333334</v>
+        <v>44755.45833333334</v>
       </c>
       <c r="B13" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="2" t="n">
-        <v>44746.5</v>
+        <v>44755.5</v>
       </c>
       <c r="B14" t="n">
         <v>0</v>
@@ -555,7 +555,7 @@
     </row>
     <row r="15">
       <c r="A15" s="2" t="n">
-        <v>44746.54166666666</v>
+        <v>44755.54166666666</v>
       </c>
       <c r="B15" t="n">
         <v>0</v>
@@ -563,7 +563,7 @@
     </row>
     <row r="16">
       <c r="A16" s="2" t="n">
-        <v>44746.58333333334</v>
+        <v>44755.58333333334</v>
       </c>
       <c r="B16" t="n">
         <v>0</v>
@@ -571,7 +571,7 @@
     </row>
     <row r="17">
       <c r="A17" s="2" t="n">
-        <v>44746.625</v>
+        <v>44755.625</v>
       </c>
       <c r="B17" t="n">
         <v>0</v>
@@ -579,7 +579,7 @@
     </row>
     <row r="18">
       <c r="A18" s="2" t="n">
-        <v>44746.66666666666</v>
+        <v>44755.66666666666</v>
       </c>
       <c r="B18" t="n">
         <v>0</v>
@@ -587,7 +587,7 @@
     </row>
     <row r="19">
       <c r="A19" s="2" t="n">
-        <v>44746.70833333334</v>
+        <v>44755.70833333334</v>
       </c>
       <c r="B19" t="n">
         <v>0</v>
@@ -595,7 +595,7 @@
     </row>
     <row r="20">
       <c r="A20" s="2" t="n">
-        <v>44746.75</v>
+        <v>44755.75</v>
       </c>
       <c r="B20" t="n">
         <v>0</v>
@@ -603,7 +603,7 @@
     </row>
     <row r="21">
       <c r="A21" s="2" t="n">
-        <v>44746.79166666666</v>
+        <v>44755.79166666666</v>
       </c>
       <c r="B21" t="n">
         <v>0</v>
@@ -611,7 +611,7 @@
     </row>
     <row r="22">
       <c r="A22" s="2" t="n">
-        <v>44746.83333333334</v>
+        <v>44755.83333333334</v>
       </c>
       <c r="B22" t="n">
         <v>0</v>
@@ -619,7 +619,7 @@
     </row>
     <row r="23">
       <c r="A23" s="2" t="n">
-        <v>44746.875</v>
+        <v>44755.875</v>
       </c>
       <c r="B23" t="n">
         <v>0</v>
@@ -627,7 +627,7 @@
     </row>
     <row r="24">
       <c r="A24" s="2" t="n">
-        <v>44746.91666666666</v>
+        <v>44755.91666666666</v>
       </c>
       <c r="B24" t="n">
         <v>0</v>
@@ -635,7 +635,7 @@
     </row>
     <row r="25">
       <c r="A25" s="2" t="n">
-        <v>44746.95833333334</v>
+        <v>44755.95833333334</v>
       </c>
       <c r="B25" t="n">
         <v>0</v>

</xml_diff>

<commit_message>
abortign error from server
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -451,7 +451,7 @@
     </row>
     <row r="2">
       <c r="A2" s="2" t="n">
-        <v>44755</v>
+        <v>44832</v>
       </c>
       <c r="B2" t="n">
         <v>0</v>
@@ -459,7 +459,7 @@
     </row>
     <row r="3">
       <c r="A3" s="2" t="n">
-        <v>44755.04166666666</v>
+        <v>44832.04166666666</v>
       </c>
       <c r="B3" t="n">
         <v>0</v>
@@ -467,7 +467,7 @@
     </row>
     <row r="4">
       <c r="A4" s="2" t="n">
-        <v>44755.08333333334</v>
+        <v>44832.08333333334</v>
       </c>
       <c r="B4" t="n">
         <v>0</v>
@@ -475,7 +475,7 @@
     </row>
     <row r="5">
       <c r="A5" s="2" t="n">
-        <v>44755.125</v>
+        <v>44832.125</v>
       </c>
       <c r="B5" t="n">
         <v>0</v>
@@ -483,7 +483,7 @@
     </row>
     <row r="6">
       <c r="A6" s="2" t="n">
-        <v>44755.16666666666</v>
+        <v>44832.16666666666</v>
       </c>
       <c r="B6" t="n">
         <v>0</v>
@@ -491,7 +491,7 @@
     </row>
     <row r="7">
       <c r="A7" s="2" t="n">
-        <v>44755.20833333334</v>
+        <v>44832.20833333334</v>
       </c>
       <c r="B7" t="n">
         <v>0</v>
@@ -499,7 +499,7 @@
     </row>
     <row r="8">
       <c r="A8" s="2" t="n">
-        <v>44755.25</v>
+        <v>44832.25</v>
       </c>
       <c r="B8" t="n">
         <v>0</v>
@@ -507,7 +507,7 @@
     </row>
     <row r="9">
       <c r="A9" s="2" t="n">
-        <v>44755.29166666666</v>
+        <v>44832.29166666666</v>
       </c>
       <c r="B9" t="n">
         <v>0</v>
@@ -515,39 +515,39 @@
     </row>
     <row r="10">
       <c r="A10" s="2" t="n">
-        <v>44755.33333333334</v>
+        <v>44832.33333333334</v>
       </c>
       <c r="B10" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="2" t="n">
-        <v>44755.375</v>
+        <v>44832.375</v>
       </c>
       <c r="B11" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="2" t="n">
-        <v>44755.41666666666</v>
+        <v>44832.41666666666</v>
       </c>
       <c r="B12" t="n">
-        <v>10</v>
+        <v>6</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="2" t="n">
-        <v>44755.45833333334</v>
+        <v>44832.45833333334</v>
       </c>
       <c r="B13" t="n">
-        <v>4</v>
+        <v>11</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="2" t="n">
-        <v>44755.5</v>
+        <v>44832.5</v>
       </c>
       <c r="B14" t="n">
         <v>0</v>
@@ -555,7 +555,7 @@
     </row>
     <row r="15">
       <c r="A15" s="2" t="n">
-        <v>44755.54166666666</v>
+        <v>44832.54166666666</v>
       </c>
       <c r="B15" t="n">
         <v>0</v>
@@ -563,7 +563,7 @@
     </row>
     <row r="16">
       <c r="A16" s="2" t="n">
-        <v>44755.58333333334</v>
+        <v>44832.58333333334</v>
       </c>
       <c r="B16" t="n">
         <v>0</v>
@@ -571,7 +571,7 @@
     </row>
     <row r="17">
       <c r="A17" s="2" t="n">
-        <v>44755.625</v>
+        <v>44832.625</v>
       </c>
       <c r="B17" t="n">
         <v>0</v>
@@ -579,7 +579,7 @@
     </row>
     <row r="18">
       <c r="A18" s="2" t="n">
-        <v>44755.66666666666</v>
+        <v>44832.66666666666</v>
       </c>
       <c r="B18" t="n">
         <v>0</v>
@@ -587,7 +587,7 @@
     </row>
     <row r="19">
       <c r="A19" s="2" t="n">
-        <v>44755.70833333334</v>
+        <v>44832.70833333334</v>
       </c>
       <c r="B19" t="n">
         <v>0</v>
@@ -595,7 +595,7 @@
     </row>
     <row r="20">
       <c r="A20" s="2" t="n">
-        <v>44755.75</v>
+        <v>44832.75</v>
       </c>
       <c r="B20" t="n">
         <v>0</v>
@@ -603,7 +603,7 @@
     </row>
     <row r="21">
       <c r="A21" s="2" t="n">
-        <v>44755.79166666666</v>
+        <v>44832.79166666666</v>
       </c>
       <c r="B21" t="n">
         <v>0</v>
@@ -611,7 +611,7 @@
     </row>
     <row r="22">
       <c r="A22" s="2" t="n">
-        <v>44755.83333333334</v>
+        <v>44832.83333333334</v>
       </c>
       <c r="B22" t="n">
         <v>0</v>
@@ -619,7 +619,7 @@
     </row>
     <row r="23">
       <c r="A23" s="2" t="n">
-        <v>44755.875</v>
+        <v>44832.875</v>
       </c>
       <c r="B23" t="n">
         <v>0</v>
@@ -627,7 +627,7 @@
     </row>
     <row r="24">
       <c r="A24" s="2" t="n">
-        <v>44755.91666666666</v>
+        <v>44832.91666666666</v>
       </c>
       <c r="B24" t="n">
         <v>0</v>
@@ -635,7 +635,7 @@
     </row>
     <row r="25">
       <c r="A25" s="2" t="n">
-        <v>44755.95833333334</v>
+        <v>44832.95833333334</v>
       </c>
       <c r="B25" t="n">
         <v>0</v>

</xml_diff>